<commit_message>
Added KLAS, updated WT/WC to v3.0
</commit_message>
<xml_diff>
--- a/excel/TS3_ACL.xlsx
+++ b/excel/TS3_ACL.xlsx
@@ -7,17 +7,19 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="KLAX_default" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="KLAX_NyergesDesign" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="KLGA_default" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="KLGA_NyergesDesign" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="KRDU_default" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="KRDU_NyergesDesign" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="OMDB_NyergesDesign" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="TIST_default" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="TIST_NyergesDesign" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="TXKF_default" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="TXKF_NyergesDesign" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="KLAS_default" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="KLAS_NyergesDesign" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="KLAX_default" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="KLAX_NyergesDesign" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="KLGA_default" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="KLGA_NyergesDesign" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="KRDU_default" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="KRDU_NyergesDesign" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="OMDB_NyergesDesign" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="TIST_default" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="TIST_NyergesDesign" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="TXKF_default" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="TXKF_NyergesDesign" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -135,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLAX_default" headerRowCount="1" id="1" name="Table_Airport_KLAX_default" ref="A1:D7">
-  <autoFilter ref="A1:D7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLAS_default" headerRowCount="1" id="1" name="Table_Airport_KLAS_default" ref="A1:D15">
+  <autoFilter ref="A1:D15"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
     <tableColumn id="2" name="Callsign"/>
@@ -148,7 +150,33 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_TXKF_default" headerRowCount="1" id="10" name="Table_Airport_TXKF_default" ref="A1:D10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_TIST_default" headerRowCount="1" id="10" name="Table_Airport_TIST_default" ref="A1:D9">
+  <autoFilter ref="A1:D9"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Airline"/>
+    <tableColumn id="2" name="Callsign"/>
+    <tableColumn id="3" name="Name"/>
+    <tableColumn id="4" name="Country Code"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_TIST_NyergesDesign" headerRowCount="1" id="11" name="Table_Airport_TIST_NyergesDesign" ref="A1:D26">
+  <autoFilter ref="A1:D26"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Airline"/>
+    <tableColumn id="2" name="Callsign"/>
+    <tableColumn id="3" name="Name"/>
+    <tableColumn id="4" name="Country Code"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_TXKF_default" headerRowCount="1" id="12" name="Table_Airport_TXKF_default" ref="A1:D10">
   <autoFilter ref="A1:D10"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
@@ -160,8 +188,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_TXKF_NyergesDesign" headerRowCount="1" id="11" name="Table_Airport_TXKF_NyergesDesign" ref="A1:D13">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_TXKF_NyergesDesign" headerRowCount="1" id="13" name="Table_Airport_TXKF_NyergesDesign" ref="A1:D13">
   <autoFilter ref="A1:D13"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
@@ -174,7 +202,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLAX_NyergesDesign" headerRowCount="1" id="2" name="Table_Airport_KLAX_NyergesDesign" ref="A1:D96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLAS_NyergesDesign" headerRowCount="1" id="2" name="Table_Airport_KLAS_NyergesDesign" ref="A1:D67">
+  <autoFilter ref="A1:D67"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Airline"/>
+    <tableColumn id="2" name="Callsign"/>
+    <tableColumn id="3" name="Name"/>
+    <tableColumn id="4" name="Country Code"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLAX_default" headerRowCount="1" id="3" name="Table_Airport_KLAX_default" ref="A1:D7">
+  <autoFilter ref="A1:D7"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Airline"/>
+    <tableColumn id="2" name="Callsign"/>
+    <tableColumn id="3" name="Name"/>
+    <tableColumn id="4" name="Country Code"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLAX_NyergesDesign" headerRowCount="1" id="4" name="Table_Airport_KLAX_NyergesDesign" ref="A1:D96">
   <autoFilter ref="A1:D96"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
@@ -186,8 +240,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLGA_default" headerRowCount="1" id="3" name="Table_Airport_KLGA_default" ref="A1:D8">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLGA_default" headerRowCount="1" id="5" name="Table_Airport_KLGA_default" ref="A1:D8">
   <autoFilter ref="A1:D8"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
@@ -199,8 +253,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLGA_NyergesDesign" headerRowCount="1" id="4" name="Table_Airport_KLGA_NyergesDesign" ref="A1:D24">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLGA_NyergesDesign" headerRowCount="1" id="6" name="Table_Airport_KLGA_NyergesDesign" ref="A1:D24">
   <autoFilter ref="A1:D24"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
@@ -212,8 +266,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KRDU_default" headerRowCount="1" id="5" name="Table_Airport_KRDU_default" ref="A1:D7">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KRDU_default" headerRowCount="1" id="7" name="Table_Airport_KRDU_default" ref="A1:D7">
   <autoFilter ref="A1:D7"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
@@ -225,8 +279,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KRDU_NyergesDesign" headerRowCount="1" id="6" name="Table_Airport_KRDU_NyergesDesign" ref="A1:D33">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KRDU_NyergesDesign" headerRowCount="1" id="8" name="Table_Airport_KRDU_NyergesDesign" ref="A1:D33">
   <autoFilter ref="A1:D33"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
@@ -238,35 +292,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_OMDB_NyergesDesign" headerRowCount="1" id="7" name="Table_Airport_OMDB_NyergesDesign" ref="A1:D86">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_OMDB_NyergesDesign" headerRowCount="1" id="9" name="Table_Airport_OMDB_NyergesDesign" ref="A1:D86">
   <autoFilter ref="A1:D86"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Airline"/>
-    <tableColumn id="2" name="Callsign"/>
-    <tableColumn id="3" name="Name"/>
-    <tableColumn id="4" name="Country Code"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_TIST_default" headerRowCount="1" id="8" name="Table_Airport_TIST_default" ref="A1:D9">
-  <autoFilter ref="A1:D9"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Airline"/>
-    <tableColumn id="2" name="Callsign"/>
-    <tableColumn id="3" name="Name"/>
-    <tableColumn id="4" name="Country Code"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_TIST_NyergesDesign" headerRowCount="1" id="9" name="Table_Airport_TIST_NyergesDesign" ref="A1:D26">
-  <autoFilter ref="A1:D26"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
     <tableColumn id="2" name="Callsign"/>
@@ -566,7 +594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,130 +633,306 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>ANG</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DENALI</t>
+          <t>GOLDSUN</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Denali Airlines</t>
+          <t>Gold Sun Air</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CAN</t>
+          <t>CHN</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FRT</t>
+          <t>BTV</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>FIELD AIR</t>
+          <t>WHITE SAND</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Feelthere International Airlines</t>
+          <t>Be There Vacation</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>BEL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LAW</t>
+          <t>CBA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LATITUDE</t>
+          <t>CHESHIRE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Latitude Airways</t>
+          <t>Chesire Blue</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NZL</t>
+          <t>GBR</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MAX</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MAGIC</t>
+          <t>DENALI</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Magic Express</t>
+          <t>Denali Airlines</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>CAN</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TAB</t>
+          <t>EMF</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LESLIE</t>
+          <t>PACKAGE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Trans American</t>
+          <t>Express Mail Freight</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>FRA</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>FRT</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FIELD AIR</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Feelthere International Airlines</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LAW</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>LATITUDE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Latitude Airways</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NZL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MAGIC</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Magic Express</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>PAV</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PATIENCE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Silent Valley Airline</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>MEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RAA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>RAINIER</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Rainier Air</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>NLD</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TAB</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LESLIE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Trans American</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TGB</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>GLOBE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Trans Global</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>DEU</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>UAX</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>OZZY</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Uluru</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>AUS</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VAL</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>VALUE</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>USA</t>
         </is>
@@ -743,6 +947,784 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
+    <col customWidth="1" max="3" min="3" width="40"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Airline</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Callsign</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Country Code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BTV</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>WHITE SAND</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Be There Vacation</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BEL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>DENALI</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Denali Airlines</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FRT</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FIELD AIR</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Feelthere International Airlines</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LAW</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>LATITUDE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Latitude Airways</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NZL</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MAGIC</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Magic Express</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TAB</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LESLIE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Trans American</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TGB</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GLOBE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Trans Global</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>DEU</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>VAL</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
+    <col customWidth="1" max="3" min="3" width="40"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Airline</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Callsign</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Country Code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AAL</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AMERICAN</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>American Airlines</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AMF</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AMFLIGHT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ameriflight</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DELTA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Delta Air Lines</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EJA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>EXECJET</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NetJets</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>EZZ</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ENTERPRIZE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>GJE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>GLOBAL JETS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GPD</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GOOD SPEED</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HPJ</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>HOP A JET</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>JBU</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>JET BLUE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>JetBlue Airways</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>JRE</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>JET SHARE</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>KAP</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CAIR</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cape Air</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>KFB</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MISSION</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>KPO</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>KRYPTO</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LXJ</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FLEXJET</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Flexjet</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>NJE</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FRACTION</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>NKS</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SPIRIT WINGS</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Spirit Airlines</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ANGUILLA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>RNI</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>RENNIA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SCX</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SUN COUNTRY</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Sun Country Airlines</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SIL</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SILVER WINGS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Silver Airways</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SNC</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NIGHT CARGO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Air Cargo Carriers</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>TJ</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>TRADEWIND</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TWY</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>TWILIGHT</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>UAL</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>UNITED</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>United Airlines</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>WAF</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>FLAMENCO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Air Flamenco</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>PRI</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -990,7 +1972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1294,6 +2276,1566 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D67"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
+    <col customWidth="1" max="3" min="3" width="40"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Airline</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Callsign</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Country Code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>AAL</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AMERICAN</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>American Airlines</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AAY</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ALLEGIANT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Allegiant Air</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ACA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AIR CANADA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Air Canada</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AMX</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AEROMEXICO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>AeroMexico</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>MEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ASA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ALASKA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alaska Airlines</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BAW</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SPEED BIRD</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>British Airways</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>GBR</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CMP</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>COPA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Copa Airlines</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DELTA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Delta Air Lines</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DAT</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DAUNTLESS</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Lynx Air</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>DOW</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DOWN TOWN</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>DRL</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DRILLER</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>EDG</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>JET EDGE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>EJA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>EXECJET</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NetJets</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>EJM</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>JET SPEED</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FEDEX</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>FEDERAL EXPRESS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>FFT</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>FRONTIER FLIGHT</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Frontier Airlines</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>FLE</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FLAIR</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Flair Airlines</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>FTH</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FOOT HILLS</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>GAJ</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>GAMA JET</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>GTI</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>GIANT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Atlas Air</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>HAL</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>HAWAIIAN</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Hawaiian Airlines</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>HRT</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CHART RIGHT</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>JBU</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>JET BLUE</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>JetBlue Airways</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>JIT</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>JET IT</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>JRE</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>JET SHARE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>JSL</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SELECT JET</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>JSX</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BIG STRIPE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>JSX (JetSuiteX)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>KAL</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>KOREAN AIR</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Korean Air</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>PRK</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>KPO</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>KRYPTO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>LET</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MEXALE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>LXJ</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>FLEXJET</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Flexjet</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>MXY</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>MOXY</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Breeze Airways</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>JET CARD</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>NKS</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SPIRIT WINGS</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Spirit Airlines</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>NOJ</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>NOVA JET</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>OKC</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>THUNDER WINGS</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>PAT</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>PAT</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>PCM</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>PAC VALLEY</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Westair Industries</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>PEG</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>PEG JET</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>QQE</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Q REX</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>ROU</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ROUGE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>AIR CANADA ROUGE</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>CAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>SCX</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SUN COUNTRY</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Sun Country Airlines</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>SJA</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SAWYER</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SKW</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>SKY WEST</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>SkyWest Airlines</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SLH</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SILVER HAWK</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SNC</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>NIGHT CARGO</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Air Cargo Carriers</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>SWA</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SOUTHWEST</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Southwest Airlines</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>TIV</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>THRIVE</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>TMB</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>VOLATO</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>TWY</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>TWILIGHT</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>UAL</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>UNITED</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>United Airlines</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>U P S</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>United Parcel Service</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>VIR</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>VIRGIN</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Virgin Atlantic Airways</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>GBR</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>VIV</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>VIAABVA</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>VivaAerobus</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>MEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>VOI</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>VOLARIS</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Volaris</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>MEX</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>VTE</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>VOLUNTEER</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>WJA</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>WEST JET</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>WestJet</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>CAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>WSN</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>WINGSPAN</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>WSP</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>WHISPER JET</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>WSW</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>SWOOP</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Swoop</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>CAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>WWI</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>WORLDWIDE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>WWW</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>XA-DON</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>XRAY ALPHA DELTA OSCAR NOVEMBER</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>XA-RFB</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>XRAY ALPHA ROMEO FOXTROT BRAVO</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>XB-NDL</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>XRAY BRAVO NOVEMBER DELTA LIMA</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>XSM</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>AIR SMART</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>GA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
+    <col customWidth="1" max="3" min="3" width="40"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Airline</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Callsign</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Country Code</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DENALI</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Denali Airlines</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FRT</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>FIELD AIR</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Feelthere International Airlines</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>LAW</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>LATITUDE</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Latitude Airways</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NZL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MAGIC</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Magic Express</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TAB</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LESLIE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Trans American</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>VAL</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3384,7 +5926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3588,7 +6130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4116,7 +6658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4298,7 +6840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5008,7 +7550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6910,782 +9452,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" width="10"/>
-    <col customWidth="1" max="2" min="2" width="25"/>
-    <col customWidth="1" max="3" min="3" width="40"/>
-    <col customWidth="1" max="4" min="4" width="15"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Airline</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Callsign</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Country Code</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>BTV</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>WHITE SAND</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Be There Vacation</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>BEL</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DEN</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>DENALI</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Denali Airlines</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FRT</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>FIELD AIR</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Feelthere International Airlines</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>LAW</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>LATITUDE</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Latitude Airways</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NZL</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>MAX</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>MAGIC</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Magic Express</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TAB</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>LESLIE</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Trans American</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>TGB</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>GLOBE</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Trans Global</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>VAL</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>VALUE</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" width="10"/>
-    <col customWidth="1" max="2" min="2" width="25"/>
-    <col customWidth="1" max="3" min="3" width="40"/>
-    <col customWidth="1" max="4" min="4" width="15"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Airline</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Callsign</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Country Code</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>AAL</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>AMERICAN</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>American Airlines</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>AMF</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>AMFLIGHT</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Ameriflight</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DAL</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>DELTA</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Delta Air Lines</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>EJA</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>EXECJET</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NetJets</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>EZZ</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ENTERPRIZE</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>GJE</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>GLOBAL JETS</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>GPD</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>GOOD SPEED</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>HPJ</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>HOP A JET</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>JBU</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>JET BLUE</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>JetBlue Airways</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>JRE</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>JET SHARE</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>KAP</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>CAIR</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Cape Air</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>KFB</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>MISSION</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>KPO</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>KRYPTO</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>LXJ</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>FLEXJET</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Flexjet</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>NJE</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>FRACTION</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>NKS</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>SPIRIT WINGS</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Spirit Airlines</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Q</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>ANGUILLA</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>RNI</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>RENNIA</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>SCX</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>SUN COUNTRY</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Sun Country Airlines</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>SIL</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>SILVER WINGS</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Silver Airways</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>SNC</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>NIGHT CARGO</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Air Cargo Carriers</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>TJ</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>TRADEWIND</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>TWY</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>TWILIGHT</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>UAL</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>UNITED</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>United Airlines</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>WAF</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>FLAMENCO</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Air Flamenco</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>PRI</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 'XRAY' to exclusion list
</commit_message>
<xml_diff>
--- a/excel/TS3_ACL.xlsx
+++ b/excel/TS3_ACL.xlsx
@@ -202,8 +202,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLAS_NyergesDesign" headerRowCount="1" id="2" name="Table_Airport_KLAS_NyergesDesign" ref="A1:D67">
-  <autoFilter ref="A1:D67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Table_Airport_KLAS_NyergesDesign" headerRowCount="1" id="2" name="Table_Airport_KLAS_NyergesDesign" ref="A1:D64">
+  <autoFilter ref="A1:D64"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Airline"/>
     <tableColumn id="2" name="Callsign"/>
@@ -2276,7 +2276,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3571,70 +3571,16 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>XA-DON</t>
+          <t>XSM</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>XRAY ALPHA DELTA OSCAR NOVEMBER</t>
+          <t>AIR SMART</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>XA-RFB</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>XRAY ALPHA ROMEO FOXTROT BRAVO</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>XB-NDL</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>XRAY BRAVO NOVEMBER DELTA LIMA</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>GA</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>XSM</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>AIR SMART</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr">
         <is>
           <t>GA</t>
         </is>

</xml_diff>

<commit_message>
#2 Update to implement full airline designator for special callsigns in GA
</commit_message>
<xml_diff>
--- a/excel/TS3_ACL.xlsx
+++ b/excel/TS3_ACL.xlsx
@@ -1537,7 +1537,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>Q3341</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2145,7 +2145,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>N842MB</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2971,7 +2971,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>N605DD</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -7301,7 +7301,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>N220CH</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">

</xml_diff>